<commit_message>
Nuevos modales y estructura del html
</commit_message>
<xml_diff>
--- a/app/cli/input/data.xlsx
+++ b/app/cli/input/data.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sando\Documents\Repositorios\Generate_msword_report\app\cli\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Banco de la Nacion\Git\PerformanceReportBN\app\cli\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DDDF74-9496-4E4A-B57C-71C6971C6905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="975" yWindow="0" windowWidth="13905" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="975" yWindow="0" windowWidth="13905" windowHeight="16200"/>
   </bookViews>
   <sheets>
     <sheet name="informe" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -270,9 +269,6 @@
   </si>
   <si>
     <t>tipo_pruebas</t>
-  </si>
-  <si>
-    <t>flujo1-carga-estrés|flujo2-estrés</t>
   </si>
   <si>
     <t>flujo1-carga -2user-60min | flujo1-estrés-hitos6-[usuarios-1,2,4,7,10,15]-[tiempo-10,10,10,10,10,10]
@@ -390,11 +386,14 @@
   <si>
     <t>Angelo Abregu</t>
   </si>
+  <si>
+    <t>flujo1-carga-estrés|flujo2-carga-estrés</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -492,8 +491,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -773,11 +772,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C4" sqref="C1:C4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,7 +904,7 @@
         <v>15</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1136,7 +1135,7 @@
         <v>66</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="120" x14ac:dyDescent="0.25">
@@ -1147,7 +1146,7 @@
         <v>67</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1155,7 +1154,7 @@
         <v>63</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>70</v>
@@ -1178,7 +1177,7 @@
         <v>75</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1197,10 +1196,10 @@
         <v>63</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1208,10 +1207,10 @@
         <v>63</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -1222,7 +1221,7 @@
         <v>68</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="210" x14ac:dyDescent="0.25">
@@ -1233,7 +1232,7 @@
         <v>69</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>